<commit_message>
Updates laptops for reals this time.
</commit_message>
<xml_diff>
--- a/public/data/laptops.xlsx
+++ b/public/data/laptops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="127">
   <si>
     <t xml:space="preserve">amazon_id</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lenovo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1920x1081</t>
   </si>
   <si>
     <t xml:space="preserve">Thin Bezel</t>
@@ -677,34 +674,33 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="37.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="65.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="116.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,7 +1093,7 @@
         <v>16</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>128</v>
@@ -1109,7 +1105,7 @@
         <v>15.6</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O7" s="0" t="n">
         <v>1.05</v>
@@ -1118,30 +1114,30 @@
         <v>5.17</v>
       </c>
       <c r="Q7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="R7" s="0" t="s">
+      <c r="S7" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="S7" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>4</v>
@@ -1150,10 +1146,10 @@
         <v>759</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>8</v>
@@ -1177,30 +1173,30 @@
         <v>5.95</v>
       </c>
       <c r="Q8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R8" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="0" t="s">
+      <c r="S8" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="S8" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="T8" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="C9" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>4</v>
@@ -1212,7 +1208,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>16</v>
@@ -1236,30 +1232,30 @@
         <v>5.82</v>
       </c>
       <c r="Q9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="R9" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="R9" s="0" t="s">
-        <v>82</v>
-      </c>
       <c r="S9" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T9" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>4.5</v>
@@ -1271,7 +1267,7 @@
         <v>53</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>16</v>
@@ -1289,7 +1285,7 @@
         <v>15.6</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O10" s="0" t="n">
         <v>0.78</v>
@@ -1298,30 +1294,30 @@
         <v>4.48</v>
       </c>
       <c r="Q10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="R10" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="R10" s="0" t="s">
+      <c r="S10" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="S10" s="0" t="s">
+      <c r="T10" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T10" s="8" t="s">
+      <c r="U10" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="U10" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>4.5</v>
@@ -1333,7 +1329,7 @@
         <v>53</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>16</v>
@@ -1342,7 +1338,7 @@
         <v>26</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>256</v>
@@ -1354,7 +1350,7 @@
         <v>15.6</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O11" s="0" t="n">
         <v>0.7</v>
@@ -1363,30 +1359,30 @@
         <v>3.96</v>
       </c>
       <c r="Q11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="R11" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="R11" s="0" t="s">
+      <c r="S11" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="S11" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="T11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="D12" s="9" t="n">
         <v>4.5</v>
@@ -1398,7 +1394,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="9" t="n">
         <v>16</v>
@@ -1407,7 +1403,7 @@
         <v>26</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K12" s="9" t="n">
         <v>1024</v>
@@ -1419,7 +1415,7 @@
         <v>15.6</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O12" s="9" t="n">
         <v>0.74</v>
@@ -1428,30 +1424,30 @@
         <v>4.49</v>
       </c>
       <c r="Q12" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="R12" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="T12" s="9" t="s">
         <v>30</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>4.5</v>
@@ -1463,7 +1459,7 @@
         <v>53</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>32</v>
@@ -1472,7 +1468,7 @@
         <v>26</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>256</v>
@@ -1484,7 +1480,7 @@
         <v>15.6</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O13" s="0" t="n">
         <v>0.7</v>
@@ -1493,27 +1489,27 @@
         <v>3.96</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R13" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="S13" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="S13" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="T13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>34</v>
@@ -1528,7 +1524,7 @@
         <v>53</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>16</v>
@@ -1537,7 +1533,7 @@
         <v>26</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>512</v>
@@ -1549,7 +1545,7 @@
         <v>15.6</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O14" s="0" t="n">
         <v>0.62</v>
@@ -1558,30 +1554,30 @@
         <v>4.63</v>
       </c>
       <c r="Q14" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="R14" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="R14" s="0" t="s">
+      <c r="S14" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="S14" s="0" t="s">
-        <v>117</v>
       </c>
       <c r="T14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>4.5</v>
@@ -1590,10 +1586,10 @@
         <v>2399</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>16</v>
@@ -1602,7 +1598,7 @@
         <v>26</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>256</v>
@@ -1614,7 +1610,7 @@
         <v>15.6</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O15" s="0" t="n">
         <v>0.7</v>
@@ -1623,27 +1619,27 @@
         <v>4.74</v>
       </c>
       <c r="Q15" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="R15" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="R15" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="S15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="T15" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T15" s="8" t="s">
+      <c r="U15" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="16" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>34</v>
@@ -1655,10 +1651,10 @@
         <v>2099</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H16" s="9" t="n">
         <v>16</v>
@@ -1667,7 +1663,7 @@
         <v>26</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K16" s="9" t="n">
         <v>512</v>
@@ -1679,7 +1675,7 @@
         <v>17.3</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O16" s="9" t="n">
         <v>0.7</v>
@@ -1688,19 +1684,19 @@
         <v>5</v>
       </c>
       <c r="Q16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="R16" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="R16" s="9" t="s">
-        <v>127</v>
-      </c>
       <c r="S16" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T16" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U16" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>